<commit_message>
correction focus clavier, bouton inutile, couleurs, annuaire de lien et début images
</commit_message>
<xml_diff>
--- a/documentation/Modèle-audit-SEO.xlsx
+++ b/documentation/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\outils_code\local_repo\VictorDauphin_4_27042021\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E147C2C0-DF8D-45C6-B60E-35F0EB15BD6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BC2ED6-3AE0-4C49-A021-CB3C5BCEBC20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="162">
   <si>
     <t>Catégorie</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>4,2:1</t>
-  </si>
-  <si>
-    <t>insufisants AA et trop petits</t>
   </si>
   <si>
     <t>insuffisant pour AA petit texte et AAA tous textes et trop petits</t>
@@ -585,12 +582,18 @@
   <si>
     <t>apporter les corrections pour avoir des titres et textes pertinents et contenant les mots-clés</t>
   </si>
+  <si>
+    <t>insufisants AAA et trop petits</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,8 +664,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +681,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -775,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -864,6 +878,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2155,7 +2187,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>5</v>
@@ -2185,22 +2217,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="D2" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="E2" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="40" t="s">
         <v>80</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" hidden="1" customHeight="1">
@@ -2208,37 +2240,37 @@
         <v>6</v>
       </c>
       <c r="B3" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="E3" s="40" t="s">
         <v>84</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>85</v>
       </c>
       <c r="F3" s="40"/>
       <c r="G3" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>96</v>
-      </c>
       <c r="F4" s="41" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
@@ -2246,60 +2278,60 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="52.5" hidden="1" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="40" t="s">
+      <c r="E6" s="41" t="s">
         <v>108</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>109</v>
       </c>
       <c r="F6" s="41"/>
     </row>
     <row r="7" spans="1:27" ht="68.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>111</v>
-      </c>
       <c r="E7" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="40.5" hidden="1" customHeight="1">
@@ -2307,74 +2339,74 @@
         <v>6</v>
       </c>
       <c r="B8" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="41" t="s">
         <v>112</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>113</v>
       </c>
       <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:27" ht="39.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="D9" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>116</v>
-      </c>
       <c r="F9" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="37.5" hidden="1" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="41" t="s">
         <v>118</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>119</v>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="34.5" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="E11" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>122</v>
-      </c>
       <c r="F11" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="44.25" hidden="1" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>123</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>124</v>
       </c>
       <c r="F12" s="41"/>
     </row>
@@ -2383,183 +2415,183 @@
         <v>6</v>
       </c>
       <c r="B13" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="E13" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="41" t="s">
-        <v>127</v>
-      </c>
       <c r="F13" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="38.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C14" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="41" t="s">
-        <v>129</v>
-      </c>
       <c r="F14" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="30.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="33" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>133</v>
-      </c>
       <c r="F16" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="33" hidden="1" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>134</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>135</v>
       </c>
       <c r="F17" s="40"/>
     </row>
     <row r="18" spans="1:6" ht="40.5" hidden="1" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="40" t="s">
         <v>136</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>137</v>
       </c>
       <c r="F18" s="40"/>
     </row>
     <row r="19" spans="1:6" ht="54.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>139</v>
-      </c>
       <c r="E19" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B20" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="D20" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="D20" s="40" t="s">
-        <v>143</v>
-      </c>
       <c r="F20" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="34.5" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="D21" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>146</v>
-      </c>
       <c r="F21" s="40" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" hidden="1" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="D22" s="40" t="s">
         <v>148</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>149</v>
       </c>
       <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6" ht="33.75" hidden="1" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>150</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>151</v>
       </c>
       <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6" ht="46.5" hidden="1" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="40" t="s">
         <v>154</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>155</v>
       </c>
       <c r="F24" s="40"/>
     </row>
@@ -3582,7 +3614,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3605,7 +3637,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -3615,7 +3647,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -3631,7 +3663,7 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3664,10 +3696,10 @@
     </row>
     <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>9</v>
@@ -3880,7 +3912,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -3951,70 +3983,70 @@
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="8"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="45"/>
     </row>
     <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="8"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="8"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6"/>
@@ -4102,7 +4134,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>26</v>
+        <v>160</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -4282,13 +4314,13 @@
     </row>
     <row r="51" spans="1:10" ht="24">
       <c r="A51" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="C51" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
@@ -4372,13 +4404,13 @@
     </row>
     <row r="58" spans="1:10" ht="30">
       <c r="A58" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -4438,13 +4470,13 @@
     </row>
     <row r="63" spans="1:10" ht="30">
       <c r="A63" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -4480,11 +4512,11 @@
     </row>
     <row r="66" spans="1:10" ht="15.75" thickBot="1">
       <c r="A66" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B66" s="15"/>
       <c r="C66" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
@@ -4497,7 +4529,7 @@
     <row r="68" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="69" spans="1:10" ht="15.75">
       <c r="A69" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -4511,10 +4543,10 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>9</v>
@@ -4529,13 +4561,13 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -4607,13 +4639,13 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B77" s="11" t="s">
-        <v>43</v>
-      </c>
       <c r="C77" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
@@ -4661,13 +4693,13 @@
     </row>
     <row r="81" spans="1:10" ht="30">
       <c r="A81" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="C81" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
@@ -4715,13 +4747,13 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -4789,43 +4821,43 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="9" spans="1:16">
       <c r="A9" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -4842,10 +4874,10 @@
     </row>
     <row r="10" spans="1:16" ht="15.75" thickBot="1">
       <c r="A10" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -4862,7 +4894,7 @@
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16">
       <c r="A14" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -4882,10 +4914,10 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -4904,10 +4936,10 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1">
       <c r="A16" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -4927,7 +4959,7 @@
     <row r="17" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="18" spans="1:6">
       <c r="A18" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -4937,7 +4969,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -5043,7 +5075,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
@@ -5115,7 +5147,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -5136,12 +5168,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5164,15 +5196,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -5184,30 +5216,30 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -5230,7 +5262,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -5251,7 +5283,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -5275,41 +5307,41 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>90</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="35" t="s">
         <v>92</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction formulaire illisible pour lecteurs, balise HTML langues, structure des titres
</commit_message>
<xml_diff>
--- a/documentation/Modèle-audit-SEO.xlsx
+++ b/documentation/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\outils_code\local_repo\VictorDauphin_4_27042021\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BC2ED6-3AE0-4C49-A021-CB3C5BCEBC20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7EAAFD-B5A3-4021-8AAC-E8B4341357BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -445,9 +445,6 @@
     <t>mauvaise structure hiérarchique des titres</t>
   </si>
   <si>
-    <t>Difficultés pour la navigation au clavier et poiur le référencement de la page</t>
-  </si>
-  <si>
     <t>revoir la structure des titres</t>
   </si>
   <si>
@@ -587,6 +584,9 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Difficultés pour la navigation au clavier et pour le référencement de la page</t>
   </si>
 </sst>
 </file>
@@ -2154,7 +2154,7 @@
   <dimension ref="A1:AA1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2187,7 +2187,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>5</v>
@@ -2229,7 +2229,7 @@
         <v>79</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G2" s="40" t="s">
         <v>80</v>
@@ -2270,7 +2270,7 @@
         <v>95</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
@@ -2290,7 +2290,7 @@
         <v>103</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>101</v>
@@ -2328,10 +2328,10 @@
         <v>110</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="40.5" hidden="1" customHeight="1">
@@ -2354,16 +2354,16 @@
         <v>113</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>72</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="37.5" hidden="1" customHeight="1">
@@ -2371,14 +2371,14 @@
         <v>106</v>
       </c>
       <c r="B10" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="41" t="s">
         <v>117</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>118</v>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="34.5" customHeight="1">
@@ -2386,16 +2386,16 @@
         <v>106</v>
       </c>
       <c r="B11" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="E11" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>121</v>
-      </c>
       <c r="F11" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="44.25" hidden="1" customHeight="1">
@@ -2403,10 +2403,10 @@
         <v>106</v>
       </c>
       <c r="B12" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>123</v>
       </c>
       <c r="F12" s="41"/>
     </row>
@@ -2415,16 +2415,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="E13" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="E13" s="41" t="s">
-        <v>126</v>
-      </c>
       <c r="F13" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="38.25" customHeight="1">
@@ -2432,16 +2432,16 @@
         <v>98</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="41" t="s">
-        <v>128</v>
-      </c>
       <c r="F14" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="30.75" customHeight="1">
@@ -2449,13 +2449,13 @@
         <v>98</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="33" customHeight="1">
@@ -2463,13 +2463,13 @@
         <v>106</v>
       </c>
       <c r="B16" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>132</v>
-      </c>
       <c r="F16" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="33" hidden="1" customHeight="1">
@@ -2477,10 +2477,10 @@
         <v>98</v>
       </c>
       <c r="B17" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>133</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>134</v>
       </c>
       <c r="F17" s="40"/>
     </row>
@@ -2489,10 +2489,10 @@
         <v>98</v>
       </c>
       <c r="B18" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="40" t="s">
         <v>135</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>136</v>
       </c>
       <c r="F18" s="40"/>
     </row>
@@ -2501,19 +2501,19 @@
         <v>98</v>
       </c>
       <c r="B19" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>138</v>
-      </c>
       <c r="E19" s="40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
@@ -2521,16 +2521,16 @@
         <v>98</v>
       </c>
       <c r="B20" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="D20" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="40" t="s">
-        <v>142</v>
-      </c>
       <c r="F20" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="34.5" customHeight="1">
@@ -2538,16 +2538,16 @@
         <v>98</v>
       </c>
       <c r="B21" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="D21" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>145</v>
-      </c>
       <c r="F21" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" hidden="1" customHeight="1">
@@ -2555,13 +2555,13 @@
         <v>98</v>
       </c>
       <c r="B22" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="D22" s="40" t="s">
         <v>147</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>148</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -2570,13 +2570,13 @@
         <v>98</v>
       </c>
       <c r="B23" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>149</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>150</v>
       </c>
       <c r="F23" s="40"/>
     </row>
@@ -2585,13 +2585,13 @@
         <v>98</v>
       </c>
       <c r="B24" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="40" t="s">
         <v>153</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>154</v>
       </c>
       <c r="F24" s="40"/>
     </row>
@@ -4134,7 +4134,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>

</xml_diff>

<commit_message>
modifications images: dimensions et balises alt, compatibilité lecteurs d'ecran, structure des titres, navigabilité globale
</commit_message>
<xml_diff>
--- a/documentation/Modèle-audit-SEO.xlsx
+++ b/documentation/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\outils_code\local_repo\VictorDauphin_4_27042021\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7EAAFD-B5A3-4021-8AAC-E8B4341357BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C551C1E-BAEA-4AC1-BAE9-BC1191BF76DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="162">
   <si>
     <t>Catégorie</t>
   </si>
@@ -424,9 +424,6 @@
     <t>SEO &amp; Accessibilité</t>
   </si>
   <si>
-    <t>Tout texte présent sur la paghe doit être visible</t>
-  </si>
-  <si>
     <t>supprimer les textes inutiles et intégrer correctement les textes utiles</t>
   </si>
   <si>
@@ -571,9 +568,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>remplacer les images par des titres et les balises adéquates</t>
-  </si>
-  <si>
     <t>Google analytics &amp; Google search console</t>
   </si>
   <si>
@@ -587,6 +581,12 @@
   </si>
   <si>
     <t>Difficultés pour la navigation au clavier et pour le référencement de la page</t>
+  </si>
+  <si>
+    <t>Tout texte présent sur la page doit être visible</t>
+  </si>
+  <si>
+    <t>remplacer les images par des titres et les balises adéquates. Configurer les balises alt des images afin de faciliter la navigatio ndes lecteurs d'ecran</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>476081</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>18988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -971,8 +971,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>157268</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>357293</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2154,7 +2154,7 @@
   <dimension ref="A1:AA1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2187,7 +2187,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>5</v>
@@ -2229,7 +2229,7 @@
         <v>79</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G2" s="40" t="s">
         <v>80</v>
@@ -2270,7 +2270,7 @@
         <v>95</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
@@ -2290,13 +2290,13 @@
         <v>103</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="52.5" hidden="1" customHeight="1">
+    <row r="6" spans="1:27" ht="52.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>106</v>
       </c>
@@ -2307,12 +2307,14 @@
         <v>105</v>
       </c>
       <c r="D6" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="41" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="7" spans="1:27" ht="68.25" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -2322,16 +2324,16 @@
         <v>64</v>
       </c>
       <c r="C7" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>110</v>
-      </c>
       <c r="E7" s="41" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="40.5" hidden="1" customHeight="1">
@@ -2339,10 +2341,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="41" t="s">
         <v>111</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>112</v>
       </c>
       <c r="F8" s="41"/>
     </row>
@@ -2351,19 +2353,19 @@
         <v>106</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>72</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="37.5" hidden="1" customHeight="1">
@@ -2371,14 +2373,14 @@
         <v>106</v>
       </c>
       <c r="B10" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="41" t="s">
         <v>116</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>117</v>
       </c>
       <c r="F10" s="41"/>
       <c r="G10" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="34.5" customHeight="1">
@@ -2386,16 +2388,16 @@
         <v>106</v>
       </c>
       <c r="B11" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="E11" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>120</v>
-      </c>
       <c r="F11" s="41" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="44.25" hidden="1" customHeight="1">
@@ -2403,10 +2405,10 @@
         <v>106</v>
       </c>
       <c r="B12" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>121</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>122</v>
       </c>
       <c r="F12" s="41"/>
     </row>
@@ -2415,16 +2417,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="E13" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="41" t="s">
-        <v>125</v>
-      </c>
       <c r="F13" s="41" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="38.25" customHeight="1">
@@ -2432,16 +2434,16 @@
         <v>98</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="41" t="s">
-        <v>127</v>
-      </c>
       <c r="F14" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="30.75" customHeight="1">
@@ -2449,13 +2451,13 @@
         <v>98</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="33" customHeight="1">
@@ -2463,13 +2465,13 @@
         <v>106</v>
       </c>
       <c r="B16" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>131</v>
-      </c>
       <c r="F16" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="33" hidden="1" customHeight="1">
@@ -2477,10 +2479,10 @@
         <v>98</v>
       </c>
       <c r="B17" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>132</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>133</v>
       </c>
       <c r="F17" s="40"/>
     </row>
@@ -2489,10 +2491,10 @@
         <v>98</v>
       </c>
       <c r="B18" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="40" t="s">
         <v>134</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>135</v>
       </c>
       <c r="F18" s="40"/>
     </row>
@@ -2501,19 +2503,19 @@
         <v>98</v>
       </c>
       <c r="B19" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>137</v>
-      </c>
       <c r="E19" s="40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
@@ -2521,16 +2523,16 @@
         <v>98</v>
       </c>
       <c r="B20" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="D20" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="D20" s="40" t="s">
-        <v>141</v>
-      </c>
       <c r="F20" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="34.5" customHeight="1">
@@ -2538,16 +2540,16 @@
         <v>98</v>
       </c>
       <c r="B21" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="D21" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>144</v>
-      </c>
       <c r="F21" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" hidden="1" customHeight="1">
@@ -2555,13 +2557,13 @@
         <v>98</v>
       </c>
       <c r="B22" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="D22" s="40" t="s">
         <v>146</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>147</v>
       </c>
       <c r="F22" s="40"/>
     </row>
@@ -2570,13 +2572,13 @@
         <v>98</v>
       </c>
       <c r="B23" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>148</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>149</v>
       </c>
       <c r="F23" s="40"/>
     </row>
@@ -2585,13 +2587,13 @@
         <v>98</v>
       </c>
       <c r="B24" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="40" t="s">
         <v>152</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>153</v>
       </c>
       <c r="F24" s="40"/>
     </row>
@@ -4134,7 +4136,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>

</xml_diff>

<commit_message>
mise à jour suivi de projet
</commit_message>
<xml_diff>
--- a/documentation/Modèle-audit-SEO.xlsx
+++ b/documentation/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\outils_code\local_repo\VictorDauphin_4_27042021\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C551C1E-BAEA-4AC1-BAE9-BC1191BF76DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBE14E2-C95C-4084-914E-EBBF9B705982}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2154,7 +2154,7 @@
   <dimension ref="A1:AA1048573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2313,7 +2313,7 @@
         <v>107</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="68.25" customHeight="1">
@@ -2457,7 +2457,7 @@
         <v>127</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="33" customHeight="1">
@@ -2471,7 +2471,7 @@
         <v>130</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="33" hidden="1" customHeight="1">
@@ -2532,7 +2532,7 @@
         <v>140</v>
       </c>
       <c r="F20" s="40" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="34.5" customHeight="1">

</xml_diff>